<commit_message>
Fix bug condominium bills (paper HP)
</commit_message>
<xml_diff>
--- a/files/inputs_FM.xlsx
+++ b/files/inputs_FM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rsericerca-my.sharepoint.com/personal/rollo_rse-web_it/Documents/Desktop/CACER - public repo/CACER-simulator/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rollo\OneDrive - RSE S.p.A\Desktop\CACER simulator - public repo\CACER-simulator\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{24024530-7E06-4182-B3E3-01B717966856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6C44FF3-6369-44B5-940F-E975C33F97D0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7716BC82-2C4C-4496-A94E-D196833EAF42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="741" activeTab="7" xr2:uid="{866B9CD4-6ADA-4356-B1C9-F1CC80F19CE1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="741" xr2:uid="{866B9CD4-6ADA-4356-B1C9-F1CC80F19CE1}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenario" sheetId="2" r:id="rId1"/>
@@ -624,9 +624,6 @@
     <t>configuration_denomination</t>
   </si>
   <si>
-    <t>CER_test_FM</t>
-  </si>
-  <si>
     <t>ITEM</t>
   </si>
   <si>
@@ -1105,6 +1102,9 @@
   </si>
   <si>
     <t>all users at month 1</t>
+  </si>
+  <si>
+    <t>AUC_paper_SDEWES</t>
   </si>
 </sst>
 </file>
@@ -1773,8 +1773,8 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1788,7 +1788,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1796,7 +1796,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>7</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1804,39 +1804,39 @@
         <v>5</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="35" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1882,7 +1882,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1900,31 +1900,31 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F1" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G1" s="15"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C2" s="9">
         <v>1</v>
@@ -1937,10 +1937,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="C3" s="9">
         <v>1</v>
@@ -1953,10 +1953,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9">
@@ -1969,10 +1969,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -1985,10 +1985,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>93</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -2001,10 +2001,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
@@ -2083,58 +2083,58 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H1" s="15"/>
       <c r="J1" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="P1" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" s="7">
         <v>1100</v>
@@ -2153,10 +2153,10 @@
       </c>
       <c r="H2" s="15"/>
       <c r="J2" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L2" s="8">
         <v>3.7499999999999999E-2</v>
@@ -2203,25 +2203,25 @@
       </c>
       <c r="H3" s="15"/>
       <c r="J3" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L3" s="8">
         <v>0.02</v>
       </c>
       <c r="M3" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N3" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="O3" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P3" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q3" s="8">
         <v>0.02</v>
@@ -2229,7 +2229,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>4</v>
@@ -2253,25 +2253,25 @@
       </c>
       <c r="H4" s="15"/>
       <c r="J4" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L4" s="4">
         <v>3</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N4" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="O4" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P4" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q4" s="4">
         <v>3</v>
@@ -2279,13 +2279,13 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D5" s="4" t="b">
         <v>0</v>
@@ -2294,24 +2294,24 @@
         <v>1</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H5" s="15"/>
       <c r="M5" s="21"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B6" s="3" t="str">
         <f>B2</f>
         <v>-</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D6" s="7">
         <f>80%*D2</f>
@@ -2322,10 +2322,10 @@
         <v>420</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H6" s="15"/>
       <c r="M6" s="21"/>
@@ -2336,42 +2336,42 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G8" s="15"/>
       <c r="H8" s="15"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="C9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H9" s="15"/>
       <c r="J9" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>2</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
@@ -2397,10 +2397,10 @@
         <v>1</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L10" s="8">
         <v>0.08</v>
@@ -2430,10 +2430,10 @@
         <v>1</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L11" s="4">
         <v>6</v>
@@ -2487,13 +2487,13 @@
         <v>1</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K13" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="L13" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
@@ -2758,13 +2758,13 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D22" s="36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E22" s="36"/>
       <c r="F22" s="20">
@@ -2786,13 +2786,13 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B23" s="7">
         <v>18000</v>
       </c>
       <c r="D23" s="36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E23" s="36"/>
       <c r="F23" s="5">
@@ -2813,7 +2813,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B24" s="7">
         <v>1000</v>
@@ -2837,13 +2837,13 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B25" s="33">
         <v>25000</v>
       </c>
       <c r="D25" s="37" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E25" s="37"/>
       <c r="F25" s="34">
@@ -2854,7 +2854,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B26" s="33">
         <v>40000</v>
@@ -2862,7 +2862,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B27" s="33">
         <v>20000</v>
@@ -2870,14 +2870,14 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B29" s="36"/>
       <c r="C29" s="5">
         <v>1.1499999999999999</v>
       </c>
       <c r="D29" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
@@ -2953,57 +2953,57 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" s="4">
         <v>18</v>
       </c>
       <c r="E2" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>146</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>147</v>
       </c>
       <c r="G2" s="4">
         <v>40</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K2" s="34">
         <v>0</v>
@@ -3011,19 +3011,19 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="4">
         <v>0.01</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G3" s="4">
         <v>1000</v>
@@ -3031,19 +3031,19 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C4" s="4">
         <v>100</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G4" s="4">
         <v>0</v>
@@ -3051,20 +3051,20 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" s="4">
         <f>2000/500</f>
         <v>4</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G5" s="4">
         <v>0</v>
@@ -3072,10 +3072,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C6" s="9">
         <v>0.01</v>
@@ -3083,10 +3083,10 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>86</v>
       </c>
       <c r="C7" s="22">
         <v>0.01</v>
@@ -3094,14 +3094,14 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="36" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B9" s="36"/>
       <c r="C9" s="5">
         <v>1.3</v>
       </c>
       <c r="D9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -3133,21 +3133,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="C2" s="4">
         <v>120</v>
@@ -3155,10 +3155,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="9">
         <v>0.1</v>
@@ -3166,10 +3166,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="C4" s="4" t="b">
         <v>1</v>
@@ -3177,7 +3177,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>4</v>
@@ -3188,10 +3188,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6" s="10">
         <v>0</v>
@@ -3199,38 +3199,38 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C7" s="10">
         <v>0.05</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" s="10">
         <v>0.1</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" s="4">
         <v>10</v>
@@ -3238,7 +3238,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="4">
@@ -3274,36 +3274,36 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="H1" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="10">
         <v>0.24</v>
@@ -3326,10 +3326,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" s="10">
         <v>3.9E-2</v>
@@ -3350,15 +3350,15 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>108</v>
       </c>
       <c r="C4" s="10">
         <v>0.23</v>
@@ -3379,15 +3379,15 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" s="10">
         <v>0.22</v>
@@ -3413,22 +3413,22 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -3468,21 +3468,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B2" s="9">
         <v>0.5</v>
@@ -3494,7 +3494,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="9">
@@ -3504,7 +3504,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
@@ -3514,7 +3514,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B5" s="9">
         <v>1</v>
@@ -3535,7 +3535,7 @@
   </sheetPr>
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -3552,33 +3552,33 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="E1" s="28" t="s">
-        <v>97</v>
-      </c>
       <c r="F1" s="26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G1" s="28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H1" s="28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -3592,7 +3592,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B3" s="9">
         <v>1</v>
@@ -3606,7 +3606,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9">
@@ -3620,7 +3620,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
@@ -3636,7 +3636,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B6" s="9">
         <v>0.3</v>
@@ -3656,7 +3656,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -3672,7 +3672,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B8" s="9">
         <v>0.1</v>
@@ -3692,7 +3692,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
@@ -3706,7 +3706,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
@@ -3724,7 +3724,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -3742,7 +3742,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B12" s="9">
         <v>0.2</v>
@@ -3760,7 +3760,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
@@ -3776,7 +3776,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -3811,10 +3811,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -3833,7 +3833,7 @@
         <v>5.7000000000000002E-2</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -3844,7 +3844,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>